<commit_message>
RF Sch, PL update
</commit_message>
<xml_diff>
--- a/1_Schematic/Build V2.0/RF-GEN-Change list_20200319.xlsx
+++ b/1_Schematic/Build V2.0/RF-GEN-Change list_20200319.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57E28CD7-B562-4249-991D-17B7A12CF74E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SET" sheetId="6" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Issue list'!$B$4:$J$4</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="245">
   <si>
     <t>No</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -877,18 +876,162 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>360pF</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>오기 수정</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C7</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>330pF</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R25, R26</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C106</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>L7, L8, L9</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.6uH/6T</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C23, C33</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>180pF</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C24, C26</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>150pF</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>330pF</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C104,C105 R8,R9</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C104,C105,C106</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>?/C-5750</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC/C-5750</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>680/2W</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R8, R9</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R25, R26</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>D1, D2, LL4148</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gate Vin 반파 정류</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C104,C105</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q2 3,4-Pin</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>snubber로 변경</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>L7,L8,L9</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0uH / 30PI</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>fc=20MHz chebyshev filter</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.6uH / 30PI / 6T</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C23,C33</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>130pF/500V</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>180pF/500V</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C24,C26</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>150pF/500V</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/30</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
     <numFmt numFmtId="177" formatCode="&quot;#&quot;00"/>
@@ -1333,7 +1476,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1792,15 +1935,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -2040,7 +2174,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2303,9 +2437,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2342,12 +2473,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2373,6 +2504,15 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="34" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2422,52 +2562,68 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="30" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="20% - 강조색1" xfId="18" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 강조색1 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - 강조색1 2" xfId="53"/>
     <cellStyle name="20% - 강조색2" xfId="22" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 강조색2 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - 강조색2 2" xfId="56"/>
     <cellStyle name="20% - 강조색3" xfId="26" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 강조색3 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="20% - 강조색3 2" xfId="59"/>
     <cellStyle name="20% - 강조색4" xfId="30" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 강조색4 2" xfId="62" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - 강조색4 2" xfId="62"/>
     <cellStyle name="20% - 강조색5" xfId="34" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 강조색5 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="20% - 강조색5 2" xfId="65"/>
     <cellStyle name="20% - 강조색6" xfId="38" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="20% - 강조색6 2" xfId="68" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="20% - 강조색6 2" xfId="68"/>
     <cellStyle name="40% - 강조색1" xfId="19" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 강조색1 2" xfId="54" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="40% - 강조색1 2" xfId="54"/>
     <cellStyle name="40% - 강조색2" xfId="23" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 강조색2 2" xfId="57" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="40% - 강조색2 2" xfId="57"/>
     <cellStyle name="40% - 강조색3" xfId="27" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 강조색3 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="40% - 강조색3 2" xfId="60"/>
     <cellStyle name="40% - 강조색4" xfId="31" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 강조색4 2" xfId="63" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="40% - 강조색4 2" xfId="63"/>
     <cellStyle name="40% - 강조색5" xfId="35" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 강조색5 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="40% - 강조색5 2" xfId="66"/>
     <cellStyle name="40% - 강조색6" xfId="39" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="40% - 강조색6 2" xfId="69" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="40% - 강조색6 2" xfId="69"/>
     <cellStyle name="60% - 강조색1" xfId="20" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 강조색1 2" xfId="45" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="60% - 강조색1 3" xfId="55" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="60% - 강조색1 2" xfId="45"/>
+    <cellStyle name="60% - 강조색1 3" xfId="55"/>
     <cellStyle name="60% - 강조색2" xfId="24" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 강조색2 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="60% - 강조색2 3" xfId="58" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="60% - 강조색2 2" xfId="46"/>
+    <cellStyle name="60% - 강조색2 3" xfId="58"/>
     <cellStyle name="60% - 강조색3" xfId="28" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 강조색3 2" xfId="47" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="60% - 강조색3 3" xfId="61" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="60% - 강조색3 2" xfId="47"/>
+    <cellStyle name="60% - 강조색3 3" xfId="61"/>
     <cellStyle name="60% - 강조색4" xfId="32" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 강조색4 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="60% - 강조색4 3" xfId="64" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="60% - 강조색4 2" xfId="48"/>
+    <cellStyle name="60% - 강조색4 3" xfId="64"/>
     <cellStyle name="60% - 강조색5" xfId="36" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 강조색5 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="60% - 강조색5 3" xfId="67" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="60% - 강조색5 2" xfId="49"/>
+    <cellStyle name="60% - 강조색5 3" xfId="67"/>
     <cellStyle name="60% - 강조색6" xfId="40" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="60% - 강조색6 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="60% - 강조색6 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="60% - 강조색6 2" xfId="50"/>
+    <cellStyle name="60% - 강조색6 3" xfId="70"/>
     <cellStyle name="강조색1" xfId="17" builtinId="29" customBuiltin="1"/>
     <cellStyle name="강조색2" xfId="21" builtinId="33" customBuiltin="1"/>
     <cellStyle name="강조색3" xfId="25" builtinId="37" customBuiltin="1"/>
@@ -2477,10 +2633,10 @@
     <cellStyle name="경고문" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="계산" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="나쁨" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="메모 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="메모 3" xfId="52" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="메모 2" xfId="42"/>
+    <cellStyle name="메모 3" xfId="52"/>
     <cellStyle name="보통" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="보통 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="보통 2" xfId="44"/>
     <cellStyle name="설명 텍스트" xfId="15" builtinId="53" customBuiltin="1"/>
     <cellStyle name="셀 확인" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="연결된 셀" xfId="12" builtinId="24" customBuiltin="1"/>
@@ -2491,12 +2647,12 @@
     <cellStyle name="제목 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="제목 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="제목 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="제목 5" xfId="43" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="제목 5" xfId="43"/>
     <cellStyle name="좋음" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="출력" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="표준 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="표준 3" xfId="51" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="표준 2" xfId="41"/>
+    <cellStyle name="표준 3" xfId="51"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -2559,7 +2715,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2592,26 +2748,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2644,23 +2783,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2836,23 +2958,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="4" max="4" width="9.5" customWidth="1"/>
-    <col min="11" max="11" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.75" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="67" t="s">
         <v>131</v>
       </c>
@@ -2860,7 +2982,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="88"/>
       <c r="C3" s="89">
         <v>1</v>
@@ -2900,7 +3022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="66" t="s">
         <v>130</v>
       </c>
@@ -2922,19 +3044,19 @@
       <c r="H4" s="64" t="s">
         <v>197</v>
       </c>
-      <c r="K4" s="115" t="s">
+      <c r="K4" s="114" t="s">
         <v>130</v>
       </c>
-      <c r="L4" s="116" t="s">
+      <c r="L4" s="115" t="s">
         <v>129</v>
       </c>
-      <c r="M4" s="117"/>
-      <c r="N4" s="117"/>
-      <c r="O4" s="117"/>
-      <c r="P4" s="117"/>
-      <c r="Q4" s="118"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.4">
+      <c r="M4" s="116"/>
+      <c r="N4" s="116"/>
+      <c r="O4" s="116"/>
+      <c r="P4" s="116"/>
+      <c r="Q4" s="117"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="57" t="s">
         <v>127</v>
       </c>
@@ -2974,14 +3096,14 @@
       <c r="P5" s="75" t="s">
         <v>185</v>
       </c>
-      <c r="Q5" s="119" t="s">
+      <c r="Q5" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="R5" s="114" t="s">
+      <c r="R5" s="113" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="77" t="s">
         <v>156</v>
       </c>
@@ -3025,7 +3147,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="62" t="s">
         <v>125</v>
       </c>
@@ -3069,7 +3191,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="57" t="s">
         <v>124</v>
       </c>
@@ -3113,7 +3235,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="57" t="s">
         <v>123</v>
       </c>
@@ -3163,7 +3285,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="57" t="s">
         <v>122</v>
       </c>
@@ -3205,7 +3327,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="57" t="s">
         <v>121</v>
       </c>
@@ -3247,7 +3369,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="57" t="s">
         <v>120</v>
       </c>
@@ -3289,7 +3411,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="57" t="s">
         <v>119</v>
       </c>
@@ -3317,7 +3439,7 @@
       <c r="L13" s="51">
         <v>100</v>
       </c>
-      <c r="M13" s="127">
+      <c r="M13" s="126">
         <v>100</v>
       </c>
       <c r="N13" s="51">
@@ -3329,11 +3451,11 @@
       <c r="P13" s="51">
         <v>100</v>
       </c>
-      <c r="Q13" s="126">
+      <c r="Q13" s="125">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="56" t="s">
         <v>118</v>
       </c>
@@ -3354,7 +3476,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="56" t="s">
         <v>117</v>
       </c>
@@ -3375,7 +3497,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" s="55" t="s">
         <v>116</v>
       </c>
@@ -3395,9 +3517,9 @@
       <c r="H16" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="L16" s="125"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="L16" s="124"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="55" t="s">
         <v>115</v>
       </c>
@@ -3418,7 +3540,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="52" t="s">
         <v>114</v>
       </c>
@@ -3439,12 +3561,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="68" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="70"/>
       <c r="C21" s="65">
         <v>1</v>
@@ -3465,7 +3587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="63"/>
       <c r="C22" s="71" t="s">
         <v>187</v>
@@ -3476,7 +3598,7 @@
       <c r="G22" s="72"/>
       <c r="H22" s="73"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="74" t="s">
         <v>190</v>
       </c>
@@ -3495,75 +3617,173 @@
       <c r="G23" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="H23" s="75" t="s">
+      <c r="H23" s="118" t="s">
         <v>191</v>
       </c>
-      <c r="I23" s="102"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B24" s="55"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="53"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B25" s="55"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="53"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B26" s="83"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="53"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B27" s="84"/>
-      <c r="C27" s="69"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="100"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B28" s="101"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="53"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B29" s="101"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="53"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B30" s="101"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="53"/>
-    </row>
-    <row r="31" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I23" s="113"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="147" t="s">
+        <v>208</v>
+      </c>
+      <c r="C24" s="148" t="s">
+        <v>209</v>
+      </c>
+      <c r="D24" s="148" t="s">
+        <v>209</v>
+      </c>
+      <c r="E24" s="148" t="s">
+        <v>209</v>
+      </c>
+      <c r="F24" s="148" t="s">
+        <v>209</v>
+      </c>
+      <c r="G24" s="148" t="s">
+        <v>209</v>
+      </c>
+      <c r="H24" s="149" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="147" t="s">
+        <v>220</v>
+      </c>
+      <c r="C25" s="148" t="s">
+        <v>210</v>
+      </c>
+      <c r="D25" s="148" t="s">
+        <v>210</v>
+      </c>
+      <c r="E25" s="148" t="s">
+        <v>210</v>
+      </c>
+      <c r="F25" s="148" t="s">
+        <v>210</v>
+      </c>
+      <c r="G25" s="148" t="s">
+        <v>210</v>
+      </c>
+      <c r="H25" s="149" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="129" t="s">
+        <v>211</v>
+      </c>
+      <c r="C26" s="148" t="s">
+        <v>210</v>
+      </c>
+      <c r="D26" s="148" t="s">
+        <v>210</v>
+      </c>
+      <c r="E26" s="148" t="s">
+        <v>210</v>
+      </c>
+      <c r="F26" s="148" t="s">
+        <v>210</v>
+      </c>
+      <c r="G26" s="148" t="s">
+        <v>210</v>
+      </c>
+      <c r="H26" s="149" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="84" t="s">
+        <v>212</v>
+      </c>
+      <c r="C27" s="54" t="s">
+        <v>210</v>
+      </c>
+      <c r="D27" s="54" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" s="54" t="s">
+        <v>210</v>
+      </c>
+      <c r="F27" s="54" t="s">
+        <v>210</v>
+      </c>
+      <c r="G27" s="54" t="s">
+        <v>210</v>
+      </c>
+      <c r="H27" s="53" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="101" t="s">
+        <v>213</v>
+      </c>
+      <c r="C28" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="D28" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="E28" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="F28" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="G28" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="H28" s="53" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="101" t="s">
+        <v>215</v>
+      </c>
+      <c r="C29" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="D29" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="E29" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="F29" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="G29" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="H29" s="53" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B30" s="101" t="s">
+        <v>217</v>
+      </c>
+      <c r="C30" s="54" t="s">
+        <v>218</v>
+      </c>
+      <c r="D30" s="54" t="s">
+        <v>218</v>
+      </c>
+      <c r="E30" s="54" t="s">
+        <v>218</v>
+      </c>
+      <c r="F30" s="54" t="s">
+        <v>218</v>
+      </c>
+      <c r="G30" s="54" t="s">
+        <v>218</v>
+      </c>
+      <c r="H30" s="53" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="77"/>
       <c r="C31" s="51"/>
       <c r="D31" s="51"/>
@@ -3572,12 +3792,12 @@
       <c r="G31" s="51"/>
       <c r="H31" s="50"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>194</v>
       </c>
@@ -3591,7 +3811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>195</v>
       </c>
@@ -3605,7 +3825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>196</v>
       </c>
@@ -3618,37 +3838,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J31"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.59765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.3984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.09765625" style="106" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="105" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="9" style="2"/>
-    <col min="7" max="7" width="43.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="2:10" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:10" s="3" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="107" t="s">
+      <c r="C4" s="106" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="14" t="s">
@@ -3673,7 +3893,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="22">
         <v>1</v>
       </c>
@@ -3702,7 +3922,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="78">
         <v>2</v>
       </c>
@@ -3727,7 +3947,7 @@
       <c r="I6" s="81"/>
       <c r="J6" s="82"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>3</v>
       </c>
@@ -3752,7 +3972,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>4</v>
       </c>
@@ -3779,11 +3999,11 @@
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="28">
         <v>5</v>
       </c>
-      <c r="C9" s="128">
+      <c r="C9" s="130">
         <v>43868</v>
       </c>
       <c r="D9" s="30" t="s">
@@ -3808,11 +4028,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="28">
         <v>6</v>
       </c>
-      <c r="C10" s="129"/>
+      <c r="C10" s="131"/>
       <c r="D10" s="30" t="s">
         <v>54</v>
       </c>
@@ -3835,11 +4055,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="28">
         <v>7</v>
       </c>
-      <c r="C11" s="130"/>
+      <c r="C11" s="132"/>
       <c r="D11" s="30" t="s">
         <v>54</v>
       </c>
@@ -3862,20 +4082,20 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="28">
         <v>8</v>
       </c>
-      <c r="C12" s="128">
+      <c r="C12" s="130">
         <v>43869</v>
       </c>
-      <c r="D12" s="103" t="s">
+      <c r="D12" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="103" t="s">
+      <c r="E12" s="102" t="s">
         <v>78</v>
       </c>
-      <c r="F12" s="103" t="s">
+      <c r="F12" s="102" t="s">
         <v>50</v>
       </c>
       <c r="G12" s="29" t="s">
@@ -3891,18 +4111,18 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="28">
         <v>9</v>
       </c>
-      <c r="C13" s="129"/>
-      <c r="D13" s="103" t="s">
+      <c r="C13" s="131"/>
+      <c r="D13" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="103" t="s">
+      <c r="E13" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="103" t="s">
+      <c r="F13" s="102" t="s">
         <v>50</v>
       </c>
       <c r="G13" s="29" t="s">
@@ -3918,18 +4138,18 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="28">
         <v>10</v>
       </c>
-      <c r="C14" s="130"/>
-      <c r="D14" s="103" t="s">
+      <c r="C14" s="132"/>
+      <c r="D14" s="102" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="103" t="s">
+      <c r="E14" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="103" t="s">
+      <c r="F14" s="102" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="29" t="s">
@@ -3945,11 +4165,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="131">
+      <c r="C15" s="133">
         <v>43870</v>
       </c>
       <c r="D15" s="85" t="s">
@@ -3972,11 +4192,11 @@
       </c>
       <c r="J15" s="33"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>12</v>
       </c>
-      <c r="C16" s="132"/>
+      <c r="C16" s="134"/>
       <c r="D16" s="5" t="s">
         <v>51</v>
       </c>
@@ -3995,11 +4215,11 @@
       <c r="I16" s="6"/>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="28">
         <v>13</v>
       </c>
-      <c r="C17" s="104">
+      <c r="C17" s="103">
         <v>43873</v>
       </c>
       <c r="D17" s="85" t="s">
@@ -4020,7 +4240,7 @@
       <c r="I17" s="29"/>
       <c r="J17" s="33"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>14</v>
       </c>
@@ -4045,32 +4265,32 @@
       <c r="I18" s="6"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="2:10" ht="52.2" x14ac:dyDescent="0.4">
-      <c r="B19" s="108">
+    <row r="19" spans="2:10" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B19" s="107">
         <v>15</v>
       </c>
-      <c r="C19" s="109">
+      <c r="C19" s="108">
         <v>43875</v>
       </c>
-      <c r="D19" s="110" t="s">
+      <c r="D19" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="110" t="s">
+      <c r="E19" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="110" t="s">
+      <c r="F19" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="111" t="s">
+      <c r="G19" s="110" t="s">
         <v>179</v>
       </c>
-      <c r="H19" s="112" t="s">
+      <c r="H19" s="111" t="s">
         <v>180</v>
       </c>
-      <c r="I19" s="112"/>
-      <c r="J19" s="113"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="I19" s="111"/>
+      <c r="J19" s="112"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
         <v>16</v>
       </c>
@@ -4093,7 +4313,7 @@
       <c r="I20" s="6"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="2:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:10" ht="33" x14ac:dyDescent="0.3">
       <c r="B21" s="4">
         <v>17</v>
       </c>
@@ -4112,15 +4332,15 @@
       <c r="G21" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="H21" s="123" t="s">
+      <c r="H21" s="122" t="s">
         <v>188</v>
       </c>
       <c r="I21" s="6"/>
-      <c r="J21" s="124" t="s">
+      <c r="J21" s="123" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="12"/>
       <c r="D22" s="5"/>
@@ -4131,7 +4351,7 @@
       <c r="I22" s="6"/>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="C23" s="12"/>
       <c r="D23" s="5"/>
@@ -4142,7 +4362,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
       <c r="C24" s="12"/>
       <c r="D24" s="5"/>
@@ -4153,7 +4373,7 @@
       <c r="I24" s="6"/>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="4"/>
       <c r="C25" s="12"/>
       <c r="D25" s="5"/>
@@ -4164,7 +4384,7 @@
       <c r="I25" s="6"/>
       <c r="J25" s="7"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
       <c r="C26" s="12"/>
       <c r="D26" s="5"/>
@@ -4175,7 +4395,7 @@
       <c r="I26" s="6"/>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="4"/>
       <c r="C27" s="12"/>
       <c r="D27" s="5"/>
@@ -4186,7 +4406,7 @@
       <c r="I27" s="6"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="4"/>
       <c r="C28" s="12"/>
       <c r="D28" s="5"/>
@@ -4197,7 +4417,7 @@
       <c r="I28" s="6"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="4"/>
       <c r="C29" s="12"/>
       <c r="D29" s="5"/>
@@ -4208,7 +4428,7 @@
       <c r="I29" s="6"/>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="4"/>
       <c r="C30" s="12"/>
       <c r="D30" s="5"/>
@@ -4219,7 +4439,7 @@
       <c r="I30" s="6"/>
       <c r="J30" s="7"/>
     </row>
-    <row r="31" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="8"/>
       <c r="C31" s="41"/>
       <c r="D31" s="9"/>
@@ -4231,7 +4451,7 @@
       <c r="J31" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="B4:J4" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="B4:J4"/>
   <mergeCells count="3">
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C12:C14"/>
@@ -4244,35 +4464,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.3984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
-    <col min="5" max="5" width="13.09765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.19921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="55.19921875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="11.3984375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="55.25" style="1" customWidth="1"/>
+    <col min="9" max="10" width="11.375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.375" style="1" customWidth="1"/>
     <col min="12" max="12" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="2:12" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:12" s="3" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="17" t="s">
         <v>0</v>
       </c>
@@ -4307,11 +4527,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="22">
         <v>1</v>
       </c>
-      <c r="C5" s="137">
+      <c r="C5" s="139">
         <v>43866</v>
       </c>
       <c r="D5" s="24">
@@ -4342,11 +4562,11 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="28">
         <v>2</v>
       </c>
-      <c r="C6" s="138"/>
+      <c r="C6" s="140"/>
       <c r="D6" s="30">
         <v>2</v>
       </c>
@@ -4375,11 +4595,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="28">
         <v>3</v>
       </c>
-      <c r="C7" s="138">
+      <c r="C7" s="140">
         <v>43868</v>
       </c>
       <c r="D7" s="30">
@@ -4410,11 +4630,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="28">
         <v>4</v>
       </c>
-      <c r="C8" s="138"/>
+      <c r="C8" s="140"/>
       <c r="D8" s="30">
         <v>1</v>
       </c>
@@ -4443,14 +4663,14 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="28">
         <v>5</v>
       </c>
-      <c r="C9" s="128">
+      <c r="C9" s="130">
         <v>43869</v>
       </c>
-      <c r="D9" s="134">
+      <c r="D9" s="136">
         <v>2</v>
       </c>
       <c r="E9" s="30" t="s">
@@ -4462,28 +4682,28 @@
       <c r="G9" s="30">
         <v>470</v>
       </c>
-      <c r="H9" s="139" t="s">
+      <c r="H9" s="141" t="s">
         <v>76</v>
       </c>
-      <c r="I9" s="133" t="s">
+      <c r="I9" s="135" t="s">
         <v>77</v>
       </c>
-      <c r="J9" s="140" t="s">
+      <c r="J9" s="142" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="133" t="s">
+      <c r="K9" s="135" t="s">
         <v>98</v>
       </c>
       <c r="L9" s="33" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="28">
         <v>6</v>
       </c>
-      <c r="C10" s="129"/>
-      <c r="D10" s="135"/>
+      <c r="C10" s="131"/>
+      <c r="D10" s="137"/>
       <c r="E10" s="30" t="s">
         <v>73</v>
       </c>
@@ -4493,20 +4713,20 @@
       <c r="G10" s="30">
         <v>47</v>
       </c>
-      <c r="H10" s="139"/>
-      <c r="I10" s="133"/>
-      <c r="J10" s="140"/>
-      <c r="K10" s="133"/>
+      <c r="H10" s="141"/>
+      <c r="I10" s="135"/>
+      <c r="J10" s="142"/>
+      <c r="K10" s="135"/>
       <c r="L10" s="33" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="28">
         <v>7</v>
       </c>
-      <c r="C11" s="129"/>
-      <c r="D11" s="135"/>
+      <c r="C11" s="131"/>
+      <c r="D11" s="137"/>
       <c r="E11" s="30" t="s">
         <v>74</v>
       </c>
@@ -4516,20 +4736,20 @@
       <c r="G11" s="30">
         <v>0</v>
       </c>
-      <c r="H11" s="139"/>
-      <c r="I11" s="133"/>
-      <c r="J11" s="140"/>
-      <c r="K11" s="133"/>
+      <c r="H11" s="141"/>
+      <c r="I11" s="135"/>
+      <c r="J11" s="142"/>
+      <c r="K11" s="135"/>
       <c r="L11" s="33" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="28">
         <v>8</v>
       </c>
-      <c r="C12" s="129"/>
-      <c r="D12" s="135"/>
+      <c r="C12" s="131"/>
+      <c r="D12" s="137"/>
       <c r="E12" s="30" t="s">
         <v>75</v>
       </c>
@@ -4539,20 +4759,20 @@
       <c r="G12" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="H12" s="139"/>
-      <c r="I12" s="133"/>
-      <c r="J12" s="140"/>
-      <c r="K12" s="133"/>
+      <c r="H12" s="141"/>
+      <c r="I12" s="135"/>
+      <c r="J12" s="142"/>
+      <c r="K12" s="135"/>
       <c r="L12" s="33" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="28">
         <v>9</v>
       </c>
-      <c r="C13" s="129"/>
-      <c r="D13" s="136"/>
+      <c r="C13" s="131"/>
+      <c r="D13" s="138"/>
       <c r="E13" s="30" t="s">
         <v>92</v>
       </c>
@@ -4562,19 +4782,19 @@
       <c r="G13" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="H13" s="139"/>
-      <c r="I13" s="133"/>
-      <c r="J13" s="140"/>
-      <c r="K13" s="133"/>
+      <c r="H13" s="141"/>
+      <c r="I13" s="135"/>
+      <c r="J13" s="142"/>
+      <c r="K13" s="135"/>
       <c r="L13" s="33" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="28">
         <v>10</v>
       </c>
-      <c r="C14" s="130"/>
+      <c r="C14" s="132"/>
       <c r="D14" s="30">
         <v>4</v>
       </c>
@@ -4603,7 +4823,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>11</v>
       </c>
@@ -4618,7 +4838,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="7"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>12</v>
       </c>
@@ -4633,7 +4853,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="7"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>13</v>
       </c>
@@ -4648,7 +4868,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="7"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>14</v>
       </c>
@@ -4663,7 +4883,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="7"/>
     </row>
-    <row r="19" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="8">
         <v>15</v>
       </c>
@@ -4696,35 +4916,35 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.3984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="11.09765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.19921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="55.19921875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="11.3984375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="55.25" style="1" customWidth="1"/>
+    <col min="9" max="10" width="11.375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.375" style="1" customWidth="1"/>
     <col min="12" max="12" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="2:12" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:12" s="3" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="17" t="s">
         <v>0</v>
       </c>
@@ -4759,11 +4979,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="22">
         <v>1</v>
       </c>
-      <c r="C5" s="141">
+      <c r="C5" s="143">
         <v>43866</v>
       </c>
       <c r="D5" s="23">
@@ -4794,11 +5014,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="28">
         <v>2</v>
       </c>
-      <c r="C6" s="130"/>
+      <c r="C6" s="132"/>
       <c r="D6" s="29">
         <v>4</v>
       </c>
@@ -4827,7 +5047,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="28">
         <v>3</v>
       </c>
@@ -4862,11 +5082,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="28">
         <v>4</v>
       </c>
-      <c r="C8" s="128">
+      <c r="C8" s="130">
         <v>43871</v>
       </c>
       <c r="D8" s="29">
@@ -4897,11 +5117,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="28">
         <v>5</v>
       </c>
-      <c r="C9" s="129"/>
+      <c r="C9" s="131"/>
       <c r="D9" s="29">
         <v>2</v>
       </c>
@@ -4914,27 +5134,27 @@
       <c r="G9" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="H9" s="142" t="s">
+      <c r="H9" s="144" t="s">
         <v>149</v>
       </c>
-      <c r="I9" s="144" t="s">
+      <c r="I9" s="146" t="s">
         <v>144</v>
       </c>
-      <c r="J9" s="144" t="s">
+      <c r="J9" s="146" t="s">
         <v>144</v>
       </c>
-      <c r="K9" s="144" t="s">
+      <c r="K9" s="146" t="s">
         <v>144</v>
       </c>
       <c r="L9" s="33" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="28">
         <v>6</v>
       </c>
-      <c r="C10" s="130"/>
+      <c r="C10" s="132"/>
       <c r="D10" s="29">
         <v>2</v>
       </c>
@@ -4947,15 +5167,15 @@
       <c r="G10" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="H10" s="143"/>
-      <c r="I10" s="136"/>
-      <c r="J10" s="136"/>
-      <c r="K10" s="136"/>
+      <c r="H10" s="145"/>
+      <c r="I10" s="138"/>
+      <c r="J10" s="138"/>
+      <c r="K10" s="138"/>
       <c r="L10" s="33" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="28">
         <v>7</v>
       </c>
@@ -4990,7 +5210,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="28">
         <v>8</v>
       </c>
@@ -5000,7 +5220,7 @@
       <c r="D12" s="29">
         <v>1</v>
       </c>
-      <c r="E12" s="121" t="s">
+      <c r="E12" s="120" t="s">
         <v>198</v>
       </c>
       <c r="F12" s="29">
@@ -5012,20 +5232,20 @@
       <c r="H12" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="I12" s="120" t="s">
+      <c r="I12" s="119" t="s">
         <v>200</v>
       </c>
-      <c r="J12" s="122" t="s">
+      <c r="J12" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="120" t="s">
+      <c r="K12" s="119" t="s">
         <v>200</v>
       </c>
       <c r="L12" s="33" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>9</v>
       </c>
@@ -5040,7 +5260,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="7"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>10</v>
       </c>
@@ -5055,7 +5275,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="7"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>11</v>
       </c>
@@ -5070,7 +5290,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="7"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>12</v>
       </c>
@@ -5085,7 +5305,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="7"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>13</v>
       </c>
@@ -5100,7 +5320,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="7"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>14</v>
       </c>
@@ -5115,7 +5335,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="7"/>
     </row>
-    <row r="19" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="4">
         <v>15</v>
       </c>
@@ -5146,35 +5366,35 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.3984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="11.09765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.19921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="55.19921875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="11.3984375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="55.25" style="1" customWidth="1"/>
+    <col min="9" max="10" width="11.375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.375" style="1" customWidth="1"/>
     <col min="12" max="12" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="2:12" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:12" s="3" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="17" t="s">
         <v>0</v>
       </c>
@@ -5209,11 +5429,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="22">
         <v>1</v>
       </c>
-      <c r="C5" s="105">
+      <c r="C5" s="104">
         <v>43874</v>
       </c>
       <c r="D5" s="23">
@@ -5242,166 +5462,276 @@
       </c>
       <c r="L5" s="27"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B6" s="4">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="28">
         <v>2</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="44">
         <v>43892</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="29">
         <v>3</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="127" t="s">
         <v>201</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B7" s="4">
+      <c r="I6" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="J6" s="152"/>
+      <c r="K6" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="L6" s="33"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="28">
         <v>3</v>
       </c>
-      <c r="C7" s="42">
-        <v>43909</v>
-      </c>
-      <c r="D7" s="6">
+      <c r="C7" s="44">
+        <v>43919</v>
+      </c>
+      <c r="D7" s="29">
         <v>2</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="127" t="s">
         <v>205</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="H7" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B8" s="4">
+      <c r="I7" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="J7" s="128" t="s">
+        <v>244</v>
+      </c>
+      <c r="K7" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="L7" s="33"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="28">
         <v>4</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="7"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B9" s="4">
+      <c r="C8" s="44"/>
+      <c r="D8" s="29">
+        <v>3</v>
+      </c>
+      <c r="E8" s="127" t="s">
+        <v>221</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="H8" s="29"/>
+      <c r="I8" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="J8" s="128" t="s">
+        <v>244</v>
+      </c>
+      <c r="K8" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="L8" s="33"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="28">
         <v>5</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="7"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B10" s="4">
+      <c r="C9" s="44"/>
+      <c r="D9" s="29">
+        <v>3</v>
+      </c>
+      <c r="E9" s="127" t="s">
+        <v>226</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="H9" s="29"/>
+      <c r="I9" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="J9" s="128" t="s">
+        <v>244</v>
+      </c>
+      <c r="K9" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="L9" s="33"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="28">
         <v>6</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B11" s="4">
+      <c r="C10" s="44"/>
+      <c r="D10" s="29">
+        <v>3</v>
+      </c>
+      <c r="E10" s="127" t="s">
+        <v>227</v>
+      </c>
+      <c r="F10" s="29">
+        <v>49.9</v>
+      </c>
+      <c r="G10" s="127" t="s">
+        <v>228</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="I10" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="J10" s="109"/>
+      <c r="K10" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="L10" s="33"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="28">
         <v>7</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B12" s="4">
+      <c r="C11" s="44"/>
+      <c r="D11" s="29">
+        <v>3</v>
+      </c>
+      <c r="E11" s="127" t="s">
+        <v>230</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>233</v>
+      </c>
+      <c r="I11" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="J11" s="109"/>
+      <c r="K11" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="L11" s="33"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="28">
         <v>8</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B13" s="4">
+      <c r="C12" s="44"/>
+      <c r="D12" s="29">
+        <v>4</v>
+      </c>
+      <c r="E12" s="127" t="s">
+        <v>234</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="H12" s="150" t="s">
+        <v>236</v>
+      </c>
+      <c r="I12" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="J12" s="128" t="s">
+        <v>244</v>
+      </c>
+      <c r="K12" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="L12" s="33"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="28">
         <v>9</v>
       </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="7"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B14" s="4">
+      <c r="C13" s="44"/>
+      <c r="D13" s="29">
+        <v>4</v>
+      </c>
+      <c r="E13" s="127" t="s">
+        <v>238</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="H13" s="151"/>
+      <c r="I13" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="J13" s="128" t="s">
+        <v>244</v>
+      </c>
+      <c r="K13" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="L13" s="33"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="28">
         <v>10</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="7"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C14" s="44"/>
+      <c r="D14" s="29">
+        <v>4</v>
+      </c>
+      <c r="E14" s="127" t="s">
+        <v>241</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="H14" s="145"/>
+      <c r="I14" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="J14" s="128" t="s">
+        <v>244</v>
+      </c>
+      <c r="K14" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="L14" s="33"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>11</v>
       </c>
@@ -5416,7 +5746,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="7"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>12</v>
       </c>
@@ -5431,7 +5761,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="7"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>13</v>
       </c>
@@ -5446,7 +5776,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="7"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>14</v>
       </c>
@@ -5461,7 +5791,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="7"/>
     </row>
-    <row r="19" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="8">
         <v>15</v>
       </c>
@@ -5477,6 +5807,9 @@
       <c r="L19" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H12:H14"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
@@ -5484,12 +5817,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>